<commit_message>
Small updates - still need to fix uncert.
</commit_message>
<xml_diff>
--- a/BubbleTrackData.xlsx
+++ b/BubbleTrackData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\opdada01\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\opdada01\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCD598DF-1EB2-4C81-AB4C-61D21A87018A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{202B490D-857F-4422-9914-8A041140061F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9525" xr2:uid="{6F0CD48B-2F8A-46BE-9EF0-089770055B17}"/>
   </bookViews>
@@ -394,7 +394,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection sqref="A1:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,7 +502,7 @@
         <v>116</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>